<commit_message>
git log and amend command added
</commit_message>
<xml_diff>
--- a/Typing practice log.xlsx
+++ b/Typing practice log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Typing practice log</t>
   </si>
@@ -34,13 +34,25 @@
   </si>
   <si>
     <t>16-21 wpm</t>
+  </si>
+  <si>
+    <t>mainly the right hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17-26 wpm</t>
+  </si>
+  <si>
+    <t>18-24 wpm</t>
+  </si>
+  <si>
+    <t>b,v.y,u,m,n,t,r,g,","</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +62,13 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -256,53 +275,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,6 +294,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,167 +628,177 @@
   <dimension ref="D2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="4:9" ht="15" customHeight="1">
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="4:9" ht="15" customHeight="1" thickBot="1">
-      <c r="E3" s="17"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="4:9" ht="15.75" thickBot="1">
-      <c r="D4" s="18"/>
+      <c r="D4" s="3"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="4:9">
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="4:9">
-      <c r="E6" s="19">
+      <c r="E6" s="12">
         <v>1</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="11" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="12"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="4:9">
-      <c r="E7" s="19">
+      <c r="E7" s="12">
         <v>2</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="4:9">
-      <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
+      <c r="E8" s="12">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="4:9">
-      <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="4:9">
-      <c r="E10" s="2"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="4:9">
-      <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="4:9">
-      <c r="E12" s="2"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="4:9">
-      <c r="E13" s="2"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="4:9">
-      <c r="E14" s="2"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="4:9">
-      <c r="E15" s="2"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="4:9">
-      <c r="E16" s="2"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="5:9">
-      <c r="E17" s="2"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="5:9">
-      <c r="E18" s="2"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="13"/>
     </row>
     <row r="19" spans="5:9">
-      <c r="E19" s="2"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="13"/>
     </row>
     <row r="20" spans="5:9">
-      <c r="E20" s="2"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="13"/>
     </row>
     <row r="21" spans="5:9">
-      <c r="E21" s="2"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="13"/>
     </row>
     <row r="22" spans="5:9" ht="15.75" thickBot="1">
-      <c r="E22" s="3"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -799,17 +828,17 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F2:H3"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
remote repository command and push command is added
</commit_message>
<xml_diff>
--- a/Typing practice log.xlsx
+++ b/Typing practice log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Typing practice log</t>
   </si>
@@ -46,6 +46,30 @@
   </si>
   <si>
     <t>b,v.y,u,m,n,t,r,g,","</t>
+  </si>
+  <si>
+    <t>20-30 wpm</t>
+  </si>
+  <si>
+    <t>y,u,o,I,b,l</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>86-91%</t>
+  </si>
+  <si>
+    <t>88-91%</t>
+  </si>
+  <si>
+    <t>90-92%</t>
+  </si>
+  <si>
+    <t>92-95%</t>
+  </si>
+  <si>
+    <t>problum in these keys is constantly deacreasing</t>
   </si>
 </sst>
 </file>
@@ -75,15 +99,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -101,45 +131,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -149,11 +143,63 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -163,110 +209,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -275,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,49 +232,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,193 +550,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:I22"/>
+  <dimension ref="A2:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="4:9" ht="15" customHeight="1">
-      <c r="F2" s="5" t="s">
+    <row r="2" spans="1:15" ht="15" customHeight="1">
+      <c r="F2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="4:9" ht="15" customHeight="1" thickBot="1">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="E3" s="2"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="4:9" ht="15.75" thickBot="1">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="D4" s="3"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="4:9">
-      <c r="E5" s="4" t="s">
+    <row r="5" spans="1:15">
+      <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="4:9">
-      <c r="E6" s="12">
+      <c r="I5" s="7"/>
+      <c r="J5" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="4:9">
-      <c r="E7" s="12">
+      <c r="I6" s="7"/>
+      <c r="J6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="E7" s="6">
         <v>2</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="4:9">
-      <c r="E8" s="12">
+      <c r="I7" s="7"/>
+      <c r="J7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="E8" s="6">
         <v>3</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="4:9">
-      <c r="E9" s="12"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="4:9">
-      <c r="E10" s="12"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="6">
+        <v>4</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="14"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickTop="1">
+      <c r="E10" s="6"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="4:9">
-      <c r="E11" s="12"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="E11" s="6"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="4:9">
-      <c r="E12" s="12"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="E12" s="6"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="4:9">
-      <c r="E13" s="12"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="E13" s="6"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="4:9">
-      <c r="E14" s="12"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="E14" s="6"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="4:9">
-      <c r="E15" s="12"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="E15" s="6"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="4:9">
-      <c r="E16" s="12"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="E16" s="6"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="5:9">
-      <c r="E17" s="12"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="5:10">
+      <c r="E17" s="6"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="5:9">
-      <c r="E18" s="12"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="5:10">
+      <c r="E18" s="6"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="5:9">
-      <c r="E19" s="12"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="5:10">
+      <c r="E19" s="6"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="5:9">
-      <c r="E20" s="12"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="5:10">
+      <c r="E20" s="6"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="5:9">
-      <c r="E21" s="12"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="5:10">
+      <c r="E21" s="6"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
+      <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="5:9" ht="15.75" thickBot="1">
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="18"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="5:10">
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F2:H3"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
@@ -828,17 +799,16 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F2:H3"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
some more branch command is added
</commit_message>
<xml_diff>
--- a/Typing practice log.xlsx
+++ b/Typing practice log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Typing practice log</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>problum in these keys is constantly deacreasing</t>
+  </si>
+  <si>
+    <t>18-25wpm</t>
+  </si>
+  <si>
+    <t>slight problum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> accuracy  was consistent</t>
+  </si>
+  <si>
+    <t>22-28wpm</t>
+  </si>
+  <si>
+    <t>minor improvement</t>
+  </si>
+  <si>
+    <t>92-94%</t>
+  </si>
+  <si>
+    <t>become more costitent</t>
   </si>
 </sst>
 </file>
@@ -113,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -158,11 +179,24 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -171,22 +205,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -194,9 +213,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="double">
@@ -206,10 +253,10 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="double">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="double">
@@ -221,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,29 +279,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,30 +613,30 @@
   <dimension ref="A2:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:15" ht="15" customHeight="1">
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="E3" s="2"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:15">
       <c r="D4" s="3"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -587,12 +647,12 @@
         <v>3</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -603,28 +663,28 @@
         <v>4</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>2</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="E8" s="6">
+    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+      <c r="E8" s="4">
         <v>3</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -635,16 +695,16 @@
         <v>9</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="6">
+    <row r="9" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4">
         <v>4</v>
       </c>
       <c r="F9" s="7" t="s">
@@ -655,123 +715,155 @@
         <v>11</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="13" t="s">
         <v>17</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
-      <c r="O9" s="14"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickTop="1">
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="O9" s="13"/>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="I10" s="7"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="J10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="E11" s="4">
+        <v>6</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="E12" s="6"/>
+      <c r="J11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickTop="1">
+      <c r="E12" s="4"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="E13" s="6"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="E14" s="6"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="E15" s="6"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="E16" s="6"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="5:10">
-      <c r="E17" s="6"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="5:10">
-      <c r="E18" s="6"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="5:10">
-      <c r="E19" s="6"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="8"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="5:10">
-      <c r="E20" s="6"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="8"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="5:10">
-      <c r="E21" s="6"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="5:10">
-      <c r="E22" s="6"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
+      <c r="J22" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="39">
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="K11:O11"/>
     <mergeCell ref="F2:H3"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F13:G13"/>

</xml_diff>